<commit_message>
refactored math validations with for loop
</commit_message>
<xml_diff>
--- a/OnlineStore/TestDataAccess/TestData.xlsx
+++ b/OnlineStore/TestDataAccess/TestData.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSet" sheetId="1" r:id="rId1"/>
+    <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="ShoppingItems" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Excel Data Source
</commit_message>
<xml_diff>
--- a/OnlineStore/TestDataAccess/TestData.xlsx
+++ b/OnlineStore/TestDataAccess/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Key</t>
   </si>
@@ -35,9 +35,6 @@
     <t>zHvsNdpj(0U$QNCF</t>
   </si>
   <si>
-    <t>.//*[@id='single_product_page_container']/div[1]/div[2]/form/div[2]/div[1]/span/input</t>
-  </si>
-  <si>
     <t>http://store.demoqa.com/products-page/product-category/accessories/magic-mouse/</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>ItemName</t>
-  </si>
-  <si>
-    <t>ItemAddToCartLocator</t>
   </si>
 </sst>
 </file>
@@ -418,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -458,10 +452,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,70 +465,52 @@
     <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>